<commit_message>
修改：添加用户 url为 /Users/:UserName 获取用户信息 url 为 /Users/:UserName
</commit_message>
<xml_diff>
--- a/UI/功能／接口设计.xlsx
+++ b/UI/功能／接口设计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="134">
   <si>
     <t>通用组件</t>
   </si>
@@ -410,10 +410,25 @@
     <t>UserName(String)</t>
   </si>
   <si>
+    <t>用户名</t>
+  </si>
+  <si>
     <t>邮箱</t>
   </si>
   <si>
     <t>用户名 唯一</t>
+  </si>
+  <si>
+    <t>/Users/:UserName</t>
+  </si>
+  <si>
+    <t>邮箱。</t>
+  </si>
+  <si>
+    <t>/Users/:UserName/Avatar</t>
+  </si>
+  <si>
+    <t>UserName</t>
   </si>
 </sst>
 </file>
@@ -1020,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="160" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1121,7 +1136,7 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>37</v>
@@ -1162,7 +1177,7 @@
         <v>68</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>68</v>
@@ -1219,7 +1234,7 @@
         <v>126</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>75</v>
@@ -1332,7 +1347,7 @@
     </row>
     <row r="22" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>91</v>
@@ -1545,7 +1560,7 @@
     </row>
     <row r="37" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>80</v>
@@ -1584,7 +1599,7 @@
         <v>68</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>69</v>
+        <v>131</v>
       </c>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -1626,92 +1641,92 @@
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>73</v>
+        <v>127</v>
       </c>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
+    <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B44" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="5" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+    <row r="45" spans="1:9" s="5" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B45" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C45" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D45" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E45" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F45" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G44" s="7" t="s">
+      <c r="G45" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H44" s="7" t="s">
+      <c r="H45" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I44" s="7" t="s">
+      <c r="I45" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
+    <row r="46" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B46" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C46" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-    </row>
-    <row r="46" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
     </row>
     <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
@@ -1723,10 +1738,10 @@
       <c r="A48" s="9"/>
       <c r="B48" s="9"/>
       <c r="C48" s="9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
@@ -1734,37 +1749,37 @@
       <c r="H48" s="9"/>
       <c r="I48" s="9"/>
     </row>
-    <row r="49" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+    <row r="49" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+    </row>
+    <row r="50" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B50" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C50" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-    </row>
-    <row r="50" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
     </row>
     <row r="51" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
@@ -1772,10 +1787,10 @@
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
       <c r="E51" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
@@ -1787,46 +1802,46 @@
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
       <c r="E52" s="9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
       <c r="I52" s="9"/>
     </row>
-    <row r="53" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
+    <row r="53" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B54" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C54" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
-    </row>
-    <row r="54" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="9"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
     </row>
     <row r="55" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="9"/>
@@ -1834,48 +1849,48 @@
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
       <c r="I55" s="9"/>
     </row>
-    <row r="56" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
+    <row r="56" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+    </row>
+    <row r="57" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B57" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C57" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8" t="s">
+      <c r="D57" s="8"/>
+      <c r="E57" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-    </row>
-    <row r="57" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="9"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F57" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
     </row>
     <row r="58" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="9"/>
@@ -1883,43 +1898,43 @@
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="E58" s="9" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
     </row>
-    <row r="59" spans="1:9" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="9"/>
-      <c r="B59" s="10"/>
+      <c r="B59" s="9"/>
       <c r="C59" s="9"/>
-      <c r="D59" s="10"/>
+      <c r="D59" s="9"/>
       <c r="E59" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+    </row>
+    <row r="60" spans="1:9" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A60" s="9"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F59" s="10" t="s">
+      <c r="F60" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="G59" s="9"/>
-      <c r="H59" s="10"/>
-      <c r="I59" s="9"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="9"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>72</v>
-      </c>
       <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
+      <c r="H60" s="10"/>
       <c r="I60" s="9"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -1928,46 +1943,46 @@
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
       <c r="E61" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
       <c r="I61" s="9"/>
     </row>
-    <row r="62" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="8" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="9"/>
+    </row>
+    <row r="63" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="B63" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="C63" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
-    </row>
-    <row r="63" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="9"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G63" s="9"/>
-      <c r="H63" s="10"/>
-      <c r="I63" s="9"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
     </row>
     <row r="64" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="9"/>
@@ -1975,87 +1990,87 @@
       <c r="C64" s="9"/>
       <c r="D64" s="10"/>
       <c r="E64" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="G64" s="9"/>
       <c r="H64" s="10"/>
       <c r="I64" s="9"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
+    <row r="65" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="9"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G65" s="9"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="9"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:9" s="5" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
+    <row r="69" spans="1:9" s="5" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B69" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C69" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D69" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="E69" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F68" s="7" t="s">
+      <c r="F69" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G68" s="7" t="s">
+      <c r="G69" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H68" s="7" t="s">
+      <c r="H69" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I68" s="7" t="s">
+      <c r="I69" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="8" t="s">
+    <row r="70" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B69" s="8" t="s">
+      <c r="B70" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="8"/>
-      <c r="H69" s="8"/>
-      <c r="I69" s="8"/>
-    </row>
-    <row r="70" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="9"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E70" s="9"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
-      <c r="I70" s="9"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
     </row>
     <row r="71" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
@@ -2067,10 +2082,10 @@
       <c r="A72" s="9"/>
       <c r="B72" s="9"/>
       <c r="C72" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
@@ -2082,10 +2097,10 @@
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
@@ -2097,16 +2112,31 @@
       <c r="A74" s="9"/>
       <c r="B74" s="9"/>
       <c r="C74" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E74" s="9"/>
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
       <c r="H74" s="9"/>
       <c r="I74" s="9"/>
+    </row>
+    <row r="75" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>